<commit_message>
KAIZEN > Typescript > Classes & Interfaces
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03722F0-0BA3-4575-92EB-26B189FCADF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7C1F2E-68AB-41A1-BF38-530C04E78D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="961" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Stack" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2623" uniqueCount="2140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="2146">
   <si>
     <t>HTML</t>
   </si>
@@ -6487,6 +6487,24 @@
   </si>
   <si>
     <t>Amazon Quicksight - Getting Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytics Tools </t>
+  </si>
+  <si>
+    <t>Amplitude</t>
+  </si>
+  <si>
+    <t>segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matomo </t>
+  </si>
+  <si>
+    <t>Sas</t>
+  </si>
+  <si>
+    <t>appsflyer</t>
   </si>
 </sst>
 </file>
@@ -6867,7 +6885,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7039,7 +7057,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7477,11 +7499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7494,9 +7516,10 @@
     <col min="7" max="7" width="39.85546875" style="7" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -7521,11 +7544,14 @@
       <c r="H1" s="92" t="s">
         <v>765</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="I1" s="95" t="s">
         <v>2108</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -7550,11 +7576,14 @@
       <c r="H2" s="93" t="s">
         <v>2067</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="96" t="s">
         <v>2109</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>0</v>
       </c>
@@ -7579,11 +7608,14 @@
       <c r="H3" s="93" t="s">
         <v>2068</v>
       </c>
-      <c r="I3" s="93" t="s">
+      <c r="I3" s="96" t="s">
         <v>2110</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -7608,11 +7640,14 @@
       <c r="H4" s="93" t="s">
         <v>2069</v>
       </c>
-      <c r="I4" s="93" t="s">
+      <c r="I4" s="96" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
@@ -7637,11 +7672,14 @@
       <c r="H5" s="93" t="s">
         <v>2070</v>
       </c>
-      <c r="I5" s="93" t="s">
+      <c r="I5" s="96" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>213</v>
       </c>
@@ -7666,11 +7704,14 @@
       <c r="H6" s="93" t="s">
         <v>2071</v>
       </c>
-      <c r="I6" s="93" t="s">
+      <c r="I6" s="96" t="s">
         <v>2113</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>214</v>
       </c>
@@ -7695,11 +7736,14 @@
       <c r="H7" s="93" t="s">
         <v>2072</v>
       </c>
-      <c r="I7" s="93" t="s">
+      <c r="I7" s="96" t="s">
         <v>2114</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>212</v>
       </c>
@@ -7724,11 +7768,11 @@
       <c r="H8" s="93" t="s">
         <v>2073</v>
       </c>
-      <c r="I8" s="93" t="s">
+      <c r="I8" s="96" t="s">
         <v>2115</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>195</v>
       </c>
@@ -7753,11 +7797,11 @@
       <c r="H9" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="93" t="s">
+      <c r="I9" s="96" t="s">
         <v>2116</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>196</v>
       </c>
@@ -7782,11 +7826,11 @@
       <c r="H10" s="93" t="s">
         <v>2074</v>
       </c>
-      <c r="I10" s="93" t="s">
+      <c r="I10" s="96" t="s">
         <v>2117</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>207</v>
       </c>
@@ -7811,11 +7855,11 @@
       <c r="H11" s="93" t="s">
         <v>2075</v>
       </c>
-      <c r="I11" s="93" t="s">
+      <c r="I11" s="96" t="s">
         <v>2118</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>208</v>
       </c>
@@ -7840,11 +7884,11 @@
       <c r="H12" s="93" t="s">
         <v>2076</v>
       </c>
-      <c r="I12" s="93" t="s">
+      <c r="I12" s="96" t="s">
         <v>2119</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>209</v>
       </c>
@@ -7869,11 +7913,11 @@
       <c r="H13" s="93" t="s">
         <v>2077</v>
       </c>
-      <c r="I13" s="93" t="s">
+      <c r="I13" s="96" t="s">
         <v>2120</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>210</v>
       </c>
@@ -7898,11 +7942,11 @@
       <c r="H14" s="93" t="s">
         <v>2078</v>
       </c>
-      <c r="I14" s="93" t="s">
+      <c r="I14" s="96" t="s">
         <v>2121</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>86</v>
       </c>
@@ -7924,11 +7968,11 @@
       <c r="H15" s="93" t="s">
         <v>2079</v>
       </c>
-      <c r="I15" s="93" t="s">
+      <c r="I15" s="96" t="s">
         <v>2122</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>88</v>
       </c>
@@ -7950,7 +7994,7 @@
       <c r="H16" s="93" t="s">
         <v>619</v>
       </c>
-      <c r="I16" s="93" t="s">
+      <c r="I16" s="96" t="s">
         <v>2123</v>
       </c>
     </row>
@@ -7976,7 +8020,7 @@
       <c r="H17" s="93" t="s">
         <v>648</v>
       </c>
-      <c r="I17" s="93" t="s">
+      <c r="I17" s="96" t="s">
         <v>2124</v>
       </c>
     </row>
@@ -7996,7 +8040,7 @@
       <c r="H18" s="93" t="s">
         <v>2080</v>
       </c>
-      <c r="I18" s="93" t="s">
+      <c r="I18" s="96" t="s">
         <v>2125</v>
       </c>
     </row>
@@ -8016,7 +8060,7 @@
       <c r="H19" s="93" t="s">
         <v>2081</v>
       </c>
-      <c r="I19" s="93" t="s">
+      <c r="I19" s="96" t="s">
         <v>2126</v>
       </c>
     </row>
@@ -8036,7 +8080,7 @@
       <c r="H20" s="93" t="s">
         <v>2082</v>
       </c>
-      <c r="I20" s="93" t="s">
+      <c r="I20" s="96" t="s">
         <v>2127</v>
       </c>
     </row>
@@ -8056,7 +8100,7 @@
       <c r="H21" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="I21" s="93" t="s">
+      <c r="I21" s="96" t="s">
         <v>2128</v>
       </c>
     </row>
@@ -8073,7 +8117,7 @@
       <c r="H22" s="93" t="s">
         <v>2083</v>
       </c>
-      <c r="I22" s="93" t="s">
+      <c r="I22" s="96" t="s">
         <v>2129</v>
       </c>
     </row>
@@ -8090,7 +8134,7 @@
       <c r="H23" s="93" t="s">
         <v>685</v>
       </c>
-      <c r="I23" s="93" t="s">
+      <c r="I23" s="96" t="s">
         <v>2130</v>
       </c>
     </row>
@@ -8107,7 +8151,7 @@
       <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="93" t="s">
+      <c r="I24" s="96" t="s">
         <v>2131</v>
       </c>
     </row>
@@ -8124,7 +8168,7 @@
       <c r="D25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="97" t="s">
         <v>2132</v>
       </c>
     </row>
@@ -8141,7 +8185,7 @@
       <c r="D26" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="93" t="s">
+      <c r="I26" s="96" t="s">
         <v>2133</v>
       </c>
     </row>
@@ -8158,7 +8202,7 @@
       <c r="D27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I27" s="93" t="s">
+      <c r="I27" s="96" t="s">
         <v>2134</v>
       </c>
     </row>
@@ -8175,7 +8219,7 @@
       <c r="D28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I28" s="93" t="s">
+      <c r="I28" s="96" t="s">
         <v>2135</v>
       </c>
     </row>
@@ -8192,7 +8236,7 @@
       <c r="D29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I29" s="93" t="s">
+      <c r="I29" s="96" t="s">
         <v>2136</v>
       </c>
     </row>
@@ -8209,7 +8253,7 @@
       <c r="D30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I30" s="93" t="s">
+      <c r="I30" s="96" t="s">
         <v>2137</v>
       </c>
     </row>
@@ -8226,7 +8270,7 @@
       <c r="D31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I31" s="93" t="s">
+      <c r="I31" s="96" t="s">
         <v>2138</v>
       </c>
     </row>
@@ -8243,7 +8287,7 @@
       <c r="D32" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I32" s="93" t="s">
+      <c r="I32" s="96" t="s">
         <v>2139</v>
       </c>
     </row>
@@ -10625,252 +10669,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>882</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
     </row>
     <row r="2" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="123" t="s">
         <v>1059</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="123"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="125"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="121" t="s">
         <v>1060</v>
       </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="120" t="s">
         <v>1061</v>
       </c>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="118"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="120"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>916</v>
       </c>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="120" t="s">
         <v>915</v>
       </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="120"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="120" t="s">
         <v>918</v>
       </c>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="118"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>919</v>
       </c>
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="120" t="s">
         <v>920</v>
       </c>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
+      <c r="C9" s="120"/>
+      <c r="D9" s="120"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>921</v>
       </c>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="120" t="s">
         <v>922</v>
       </c>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="118"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="120" t="s">
         <v>924</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="120" t="s">
         <v>926</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>1062</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="120" t="s">
         <v>1065</v>
       </c>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>1063</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="120" t="s">
         <v>1066</v>
       </c>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>1064</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="120" t="s">
         <v>1067</v>
       </c>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="B16" s="118" t="s">
+      <c r="B16" s="120" t="s">
         <v>928</v>
       </c>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="130"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="132"/>
+      <c r="A17" s="132"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="134"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="127"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
-      <c r="I18" s="129"/>
+      <c r="A18" s="129"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="130"/>
+      <c r="I18" s="131"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="55" t="s">
@@ -11050,17 +11094,17 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="124" t="s">
+      <c r="A56" s="126" t="s">
         <v>930</v>
       </c>
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
-      <c r="D56" s="125"/>
-      <c r="E56" s="125"/>
-      <c r="F56" s="125"/>
-      <c r="G56" s="125"/>
-      <c r="H56" s="125"/>
-      <c r="I56" s="126"/>
+      <c r="B56" s="127"/>
+      <c r="C56" s="127"/>
+      <c r="D56" s="127"/>
+      <c r="E56" s="127"/>
+      <c r="F56" s="127"/>
+      <c r="G56" s="127"/>
+      <c r="H56" s="127"/>
+      <c r="I56" s="128"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="51" t="s">
@@ -11530,16 +11574,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="136"/>
+      <c r="C1" s="138"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="139" t="s">
         <v>406</v>
       </c>
-      <c r="C2" s="138"/>
+      <c r="C2" s="140"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
@@ -11597,10 +11641,10 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="137" t="s">
+      <c r="B15" s="139" t="s">
         <v>407</v>
       </c>
-      <c r="C15" s="138"/>
+      <c r="C15" s="140"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
@@ -11770,10 +11814,10 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="137" t="s">
+      <c r="B50" s="139" t="s">
         <v>408</v>
       </c>
-      <c r="C50" s="138"/>
+      <c r="C50" s="140"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="25" t="s">
@@ -11861,10 +11905,10 @@
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="139" t="s">
+      <c r="B69" s="141" t="s">
         <v>409</v>
       </c>
-      <c r="C69" s="140"/>
+      <c r="C69" s="142"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="25" t="s">
@@ -11882,10 +11926,10 @@
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="139" t="s">
+      <c r="B74" s="141" t="s">
         <v>410</v>
       </c>
-      <c r="C74" s="140"/>
+      <c r="C74" s="142"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="19" t="s">
@@ -12002,10 +12046,10 @@
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="137" t="s">
+      <c r="B98" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="C98" s="138"/>
+      <c r="C98" s="140"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="25" t="s">
@@ -12039,10 +12083,10 @@
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="137" t="s">
+      <c r="B106" s="139" t="s">
         <v>412</v>
       </c>
-      <c r="C106" s="138"/>
+      <c r="C106" s="140"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="25" t="s">
@@ -12108,10 +12152,10 @@
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="137" t="s">
+      <c r="B120" s="139" t="s">
         <v>413</v>
       </c>
-      <c r="C120" s="138"/>
+      <c r="C120" s="140"/>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="25" t="s">
@@ -12124,10 +12168,10 @@
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="133" t="s">
+      <c r="B124" s="135" t="s">
         <v>414</v>
       </c>
-      <c r="C124" s="135"/>
+      <c r="C124" s="137"/>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="25" t="s">
@@ -12226,10 +12270,10 @@
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="133" t="s">
+      <c r="B138" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="C138" s="135"/>
+      <c r="C138" s="137"/>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="25" t="s">
@@ -12296,10 +12340,10 @@
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="133" t="s">
+      <c r="B148" s="135" t="s">
         <v>416</v>
       </c>
-      <c r="C148" s="134"/>
+      <c r="C148" s="136"/>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="25" t="s">
@@ -12550,10 +12594,10 @@
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" s="133" t="s">
+      <c r="B181" s="135" t="s">
         <v>417</v>
       </c>
-      <c r="C181" s="135"/>
+      <c r="C181" s="137"/>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="25" t="s">
@@ -12676,10 +12720,10 @@
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="133" t="s">
+      <c r="A198" s="135" t="s">
         <v>418</v>
       </c>
-      <c r="B198" s="134"/>
+      <c r="B198" s="136"/>
       <c r="C198" s="38" t="s">
         <v>726</v>
       </c>
@@ -15299,7 +15343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15E8F75-5B0F-4CE7-B0CE-45D9E5D1F43A}">
   <dimension ref="A1:C277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:A10"/>
     </sheetView>
@@ -15312,10 +15356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>646</v>
       </c>
-      <c r="B1" s="97"/>
+      <c r="B1" s="99"/>
       <c r="C1" s="9" t="s">
         <v>2066</v>
       </c>
@@ -17271,10 +17315,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="143" t="s">
         <v>540</v>
       </c>
-      <c r="B1" s="141"/>
+      <c r="B1" s="143"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -17450,10 +17494,10 @@
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="144" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="143"/>
+      <c r="C1" s="145"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -17660,10 +17704,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="146" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="144"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="11" t="s">
         <v>226</v>
       </c>
@@ -17675,7 +17719,7 @@
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="145">
+      <c r="C2" s="147">
         <v>0.2</v>
       </c>
     </row>
@@ -17686,7 +17730,7 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="146"/>
+      <c r="C3" s="148"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -17788,24 +17832,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="D1" s="117" t="s">
+      <c r="B1" s="119"/>
+      <c r="D1" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="117"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="149" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="D2" s="147" t="s">
+      <c r="B2" s="149"/>
+      <c r="D2" s="149" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="147"/>
+      <c r="E2" s="149"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -17976,14 +18020,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="147" t="s">
+      <c r="A16" s="149" t="s">
         <v>262</v>
       </c>
-      <c r="B16" s="147"/>
-      <c r="D16" s="147" t="s">
+      <c r="B16" s="149"/>
+      <c r="D16" s="149" t="s">
         <v>341</v>
       </c>
-      <c r="E16" s="147"/>
+      <c r="E16" s="149"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -18154,14 +18198,14 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="147" t="s">
+      <c r="A30" s="149" t="s">
         <v>275</v>
       </c>
-      <c r="B30" s="147"/>
-      <c r="D30" s="147" t="s">
+      <c r="B30" s="149"/>
+      <c r="D30" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="E30" s="147"/>
+      <c r="E30" s="149"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -18332,14 +18376,14 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="147" t="s">
+      <c r="A44" s="149" t="s">
         <v>288</v>
       </c>
-      <c r="B44" s="147"/>
-      <c r="D44" s="147" t="s">
+      <c r="B44" s="149"/>
+      <c r="D44" s="149" t="s">
         <v>367</v>
       </c>
-      <c r="E44" s="147"/>
+      <c r="E44" s="149"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -18510,14 +18554,14 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="147" t="s">
+      <c r="A58" s="149" t="s">
         <v>301</v>
       </c>
-      <c r="B58" s="147"/>
-      <c r="D58" s="147" t="s">
+      <c r="B58" s="149"/>
+      <c r="D58" s="149" t="s">
         <v>380</v>
       </c>
-      <c r="E58" s="147"/>
+      <c r="E58" s="149"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
@@ -18691,14 +18735,14 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="147" t="s">
+      <c r="A72" s="149" t="s">
         <v>315</v>
       </c>
-      <c r="B72" s="147"/>
-      <c r="D72" s="147" t="s">
+      <c r="B72" s="149"/>
+      <c r="D72" s="149" t="s">
         <v>393</v>
       </c>
-      <c r="E72" s="147"/>
+      <c r="E72" s="149"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -18935,7 +18979,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="112" t="s">
         <v>160</v>
       </c>
       <c r="B4" s="61" t="s">
@@ -18943,8 +18987,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="113" t="s">
+      <c r="A5" s="113"/>
+      <c r="B5" s="115" t="s">
         <v>1692</v>
       </c>
       <c r="C5" s="62" t="s">
@@ -18952,37 +18996,37 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="113"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="62" t="s">
         <v>1694</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="111"/>
-      <c r="B7" s="113"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="62" t="s">
         <v>1695</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="111"/>
-      <c r="B8" s="113"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="115"/>
       <c r="C8" s="62" t="s">
         <v>1696</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
-      <c r="B9" s="113"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="115"/>
       <c r="C9" s="62" t="s">
         <v>1697</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="111"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="114" t="s">
+      <c r="A10" s="113"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="116" t="s">
         <v>1698</v>
       </c>
       <c r="D10" s="63" t="s">
@@ -18990,135 +19034,135 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="111"/>
-      <c r="B11" s="113"/>
-      <c r="C11" s="114"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="115"/>
+      <c r="C11" s="116"/>
       <c r="D11" s="63" t="s">
         <v>1695</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="114"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="116"/>
       <c r="D12" s="63" t="s">
         <v>1696</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="114"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="63" t="s">
         <v>1697</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="111"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="114"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="116"/>
       <c r="D14" s="63" t="s">
         <v>1700</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="61" t="s">
         <v>1701</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="111"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="61" t="s">
         <v>1702</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="61" t="s">
         <v>1703</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="111"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="61" t="s">
         <v>1704</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
+      <c r="A19" s="113"/>
       <c r="B19" s="61" t="s">
         <v>1705</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="111"/>
+      <c r="A20" s="113"/>
       <c r="B20" s="61" t="s">
         <v>1706</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="111"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="61" t="s">
         <v>1707</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="61" t="s">
         <v>1708</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="111"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="61" t="s">
         <v>1709</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
+      <c r="A24" s="113"/>
       <c r="B24" s="61" t="s">
         <v>1710</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="111"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="61" t="s">
         <v>1711</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="111"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="61" t="s">
         <v>1712</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="111"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="61" t="s">
         <v>1713</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="111"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="61" t="s">
         <v>1714</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="111"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="61" t="s">
         <v>1715</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="112"/>
+      <c r="A30" s="114"/>
       <c r="B30" s="61" t="s">
         <v>1716</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="110" t="s">
+      <c r="A31" s="112" t="s">
         <v>1717</v>
       </c>
       <c r="B31" s="61" t="s">
@@ -19126,67 +19170,67 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="111"/>
+      <c r="A32" s="113"/>
       <c r="B32" s="61" t="s">
         <v>1718</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
+      <c r="A33" s="113"/>
       <c r="B33" s="61" t="s">
         <v>1719</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="111"/>
+      <c r="A34" s="113"/>
       <c r="B34" s="61" t="s">
         <v>1720</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
+      <c r="A35" s="113"/>
       <c r="B35" s="61" t="s">
         <v>1721</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="111"/>
+      <c r="A36" s="113"/>
       <c r="B36" s="61" t="s">
         <v>1550</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
+      <c r="A37" s="113"/>
       <c r="B37" s="61" t="s">
         <v>1722</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="111"/>
+      <c r="A38" s="113"/>
       <c r="B38" s="61" t="s">
         <v>1723</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
+      <c r="A39" s="113"/>
       <c r="B39" s="61" t="s">
         <v>1724</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="111"/>
+      <c r="A40" s="113"/>
       <c r="B40" s="61" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="112"/>
+      <c r="A41" s="114"/>
       <c r="B41" s="61" t="s">
         <v>1726</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="110" t="s">
+      <c r="A42" s="112" t="s">
         <v>1727</v>
       </c>
       <c r="B42" s="61" t="s">
@@ -19194,61 +19238,61 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
+      <c r="A43" s="113"/>
       <c r="B43" s="61" t="s">
         <v>1728</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="111"/>
+      <c r="A44" s="113"/>
       <c r="B44" s="61" t="s">
         <v>1730</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
+      <c r="A45" s="113"/>
       <c r="B45" s="61" t="s">
         <v>1731</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="61" t="s">
         <v>1732</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="111"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="61" t="s">
         <v>1733</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="61" t="s">
         <v>1734</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
+      <c r="A49" s="113"/>
       <c r="B49" s="61" t="s">
         <v>1735</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="111"/>
+      <c r="A50" s="113"/>
       <c r="B50" s="61" t="s">
         <v>1736</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="112"/>
+      <c r="A51" s="114"/>
       <c r="B51" s="61" t="s">
         <v>1737</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="110" t="s">
+      <c r="A52" s="112" t="s">
         <v>1738</v>
       </c>
       <c r="B52" s="61" t="s">
@@ -19256,104 +19300,104 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="111"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="61" t="s">
         <v>1740</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="111"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="61" t="s">
         <v>1741</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="111"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="61" t="s">
         <v>1742</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="111"/>
+      <c r="A56" s="113"/>
       <c r="B56" s="61" t="s">
         <v>1743</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="111"/>
+      <c r="A57" s="113"/>
       <c r="B57" s="61" t="s">
         <v>1744</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="111"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="61" t="s">
         <v>1722</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="111"/>
+      <c r="A59" s="113"/>
       <c r="B59" s="61" t="s">
         <v>1745</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="111"/>
+      <c r="A60" s="113"/>
       <c r="B60" s="61" t="s">
         <v>1746</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="111"/>
+      <c r="A61" s="113"/>
       <c r="B61" s="61" t="s">
         <v>1724</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="111"/>
+      <c r="A62" s="113"/>
       <c r="B62" s="61" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="111"/>
+      <c r="A63" s="113"/>
       <c r="B63" s="61" t="s">
         <v>1747</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="111"/>
+      <c r="A64" s="113"/>
       <c r="B64" s="61" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="111"/>
+      <c r="A65" s="113"/>
       <c r="B65" s="61" t="s">
         <v>1748</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="111"/>
+      <c r="A66" s="113"/>
       <c r="B66" s="61" t="s">
         <v>1749</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="111"/>
+      <c r="A67" s="113"/>
       <c r="B67" s="61" t="s">
         <v>1750</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="111"/>
+      <c r="A68" s="113"/>
       <c r="B68" s="61" t="s">
         <v>1645</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="111"/>
-      <c r="B69" s="104" t="s">
+      <c r="A69" s="113"/>
+      <c r="B69" s="106" t="s">
         <v>1751</v>
       </c>
       <c r="C69" s="62" t="s">
@@ -19361,57 +19405,57 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="111"/>
-      <c r="B70" s="105"/>
+      <c r="A70" s="113"/>
+      <c r="B70" s="107"/>
       <c r="C70" s="62" t="s">
         <v>1753</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="111"/>
-      <c r="B71" s="105"/>
+      <c r="A71" s="113"/>
+      <c r="B71" s="107"/>
       <c r="C71" s="62" t="s">
         <v>1754</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="111"/>
-      <c r="B72" s="105"/>
+      <c r="A72" s="113"/>
+      <c r="B72" s="107"/>
       <c r="C72" s="62" t="s">
         <v>1755</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="111"/>
-      <c r="B73" s="105"/>
+      <c r="A73" s="113"/>
+      <c r="B73" s="107"/>
       <c r="C73" s="62" t="s">
         <v>1756</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
-      <c r="B74" s="105"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="107"/>
       <c r="C74" s="62" t="s">
         <v>1757</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
-      <c r="B75" s="105"/>
+      <c r="A75" s="113"/>
+      <c r="B75" s="107"/>
       <c r="C75" s="62" t="s">
         <v>1758</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="111"/>
-      <c r="B76" s="106"/>
+      <c r="A76" s="113"/>
+      <c r="B76" s="108"/>
       <c r="C76" s="62" t="s">
         <v>1759</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="111"/>
-      <c r="B77" s="104" t="s">
+      <c r="A77" s="113"/>
+      <c r="B77" s="106" t="s">
         <v>1760</v>
       </c>
       <c r="C77" s="62" t="s">
@@ -19419,145 +19463,145 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="111"/>
-      <c r="B78" s="105"/>
+      <c r="A78" s="113"/>
+      <c r="B78" s="107"/>
       <c r="C78" s="62" t="s">
         <v>1762</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="111"/>
-      <c r="B79" s="105"/>
+      <c r="A79" s="113"/>
+      <c r="B79" s="107"/>
       <c r="C79" s="62" t="s">
         <v>1763</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="111"/>
-      <c r="B80" s="105"/>
+      <c r="A80" s="113"/>
+      <c r="B80" s="107"/>
       <c r="C80" s="62" t="s">
         <v>1764</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="111"/>
-      <c r="B81" s="105"/>
+      <c r="A81" s="113"/>
+      <c r="B81" s="107"/>
       <c r="C81" s="62" t="s">
         <v>1765</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="111"/>
-      <c r="B82" s="105"/>
+      <c r="A82" s="113"/>
+      <c r="B82" s="107"/>
       <c r="C82" s="62" t="s">
         <v>1766</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="111"/>
-      <c r="B83" s="105"/>
+      <c r="A83" s="113"/>
+      <c r="B83" s="107"/>
       <c r="C83" s="62" t="s">
         <v>1767</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="111"/>
-      <c r="B84" s="105"/>
+      <c r="A84" s="113"/>
+      <c r="B84" s="107"/>
       <c r="C84" s="62" t="s">
         <v>1768</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
-      <c r="B85" s="105"/>
+      <c r="A85" s="113"/>
+      <c r="B85" s="107"/>
       <c r="C85" s="62" t="s">
         <v>1769</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="111"/>
-      <c r="B86" s="105"/>
+      <c r="A86" s="113"/>
+      <c r="B86" s="107"/>
       <c r="C86" s="62" t="s">
         <v>1770</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="111"/>
-      <c r="B87" s="105"/>
+      <c r="A87" s="113"/>
+      <c r="B87" s="107"/>
       <c r="C87" s="62" t="s">
         <v>1771</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="111"/>
-      <c r="B88" s="105"/>
+      <c r="A88" s="113"/>
+      <c r="B88" s="107"/>
       <c r="C88" s="62" t="s">
         <v>1772</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="111"/>
-      <c r="B89" s="105"/>
+      <c r="A89" s="113"/>
+      <c r="B89" s="107"/>
       <c r="C89" s="62" t="s">
         <v>1773</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="111"/>
-      <c r="B90" s="105"/>
+      <c r="A90" s="113"/>
+      <c r="B90" s="107"/>
       <c r="C90" s="62" t="s">
         <v>1774</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="111"/>
-      <c r="B91" s="105"/>
+      <c r="A91" s="113"/>
+      <c r="B91" s="107"/>
       <c r="C91" s="62" t="s">
         <v>1775</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="111"/>
-      <c r="B92" s="105"/>
+      <c r="A92" s="113"/>
+      <c r="B92" s="107"/>
       <c r="C92" s="62" t="s">
         <v>1776</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="111"/>
-      <c r="B93" s="105"/>
+      <c r="A93" s="113"/>
+      <c r="B93" s="107"/>
       <c r="C93" s="62" t="s">
         <v>1777</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="111"/>
-      <c r="B94" s="106"/>
+      <c r="A94" s="113"/>
+      <c r="B94" s="108"/>
       <c r="C94" s="62" t="s">
         <v>1778</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="111"/>
+      <c r="A95" s="113"/>
       <c r="B95" s="61" t="s">
         <v>1779</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="111"/>
+      <c r="A96" s="113"/>
       <c r="B96" s="61" t="s">
         <v>1780</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="111"/>
+      <c r="A97" s="113"/>
       <c r="B97" s="61" t="s">
         <v>1781</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="111"/>
-      <c r="B98" s="104" t="s">
+      <c r="A98" s="113"/>
+      <c r="B98" s="106" t="s">
         <v>1782</v>
       </c>
       <c r="C98" s="62" t="s">
@@ -19565,81 +19609,81 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="111"/>
-      <c r="B99" s="105"/>
+      <c r="A99" s="113"/>
+      <c r="B99" s="107"/>
       <c r="C99" s="62" t="s">
         <v>1784</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="111"/>
-      <c r="B100" s="105"/>
+      <c r="A100" s="113"/>
+      <c r="B100" s="107"/>
       <c r="C100" s="62" t="s">
         <v>1785</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="111"/>
-      <c r="B101" s="105"/>
+      <c r="A101" s="113"/>
+      <c r="B101" s="107"/>
       <c r="C101" s="62" t="s">
         <v>1782</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="111"/>
-      <c r="B102" s="105"/>
+      <c r="A102" s="113"/>
+      <c r="B102" s="107"/>
       <c r="C102" s="62" t="s">
         <v>1786</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="111"/>
-      <c r="B103" s="105"/>
+      <c r="A103" s="113"/>
+      <c r="B103" s="107"/>
       <c r="C103" s="62" t="s">
         <v>1787</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="111"/>
-      <c r="B104" s="105"/>
+      <c r="A104" s="113"/>
+      <c r="B104" s="107"/>
       <c r="C104" s="62" t="s">
         <v>1788</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="111"/>
-      <c r="B105" s="105"/>
+      <c r="A105" s="113"/>
+      <c r="B105" s="107"/>
       <c r="C105" s="62" t="s">
         <v>1789</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="111"/>
-      <c r="B106" s="106"/>
+      <c r="A106" s="113"/>
+      <c r="B106" s="108"/>
       <c r="C106" s="62" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="111"/>
+      <c r="A107" s="113"/>
       <c r="B107" s="61" t="s">
         <v>1790</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="111"/>
+      <c r="A108" s="113"/>
       <c r="B108" s="61" t="s">
         <v>1791</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="112"/>
+      <c r="A109" s="114"/>
       <c r="B109" s="61" t="s">
         <v>1792</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="110" t="s">
+      <c r="A110" s="112" t="s">
         <v>1793</v>
       </c>
       <c r="B110" s="61" t="s">
@@ -19647,49 +19691,49 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="111"/>
+      <c r="A111" s="113"/>
       <c r="B111" s="61" t="s">
         <v>1795</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="111"/>
+      <c r="A112" s="113"/>
       <c r="B112" s="61" t="s">
         <v>1796</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="111"/>
+      <c r="A113" s="113"/>
       <c r="B113" s="61" t="s">
         <v>1797</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="111"/>
+      <c r="A114" s="113"/>
       <c r="B114" s="61" t="s">
         <v>1798</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="111"/>
+      <c r="A115" s="113"/>
       <c r="B115" s="61" t="s">
         <v>1799</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="111"/>
+      <c r="A116" s="113"/>
       <c r="B116" s="61" t="s">
         <v>1800</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="112"/>
+      <c r="A117" s="114"/>
       <c r="B117" s="61" t="s">
         <v>1801</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="110" t="s">
+      <c r="A118" s="112" t="s">
         <v>1802</v>
       </c>
       <c r="B118" s="61" t="s">
@@ -19697,38 +19741,38 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="111"/>
+      <c r="A119" s="113"/>
       <c r="B119" s="61" t="s">
         <v>1804</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="111"/>
+      <c r="A120" s="113"/>
       <c r="B120" s="61" t="s">
         <v>1805</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="111"/>
+      <c r="A121" s="113"/>
       <c r="B121" s="61" t="s">
         <v>1806</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="111"/>
+      <c r="A122" s="113"/>
       <c r="B122" s="61" t="s">
         <v>1807</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="111"/>
+      <c r="A123" s="113"/>
       <c r="B123" s="61" t="s">
         <v>1808</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="111"/>
-      <c r="B124" s="104" t="s">
+      <c r="A124" s="113"/>
+      <c r="B124" s="106" t="s">
         <v>1809</v>
       </c>
       <c r="C124" s="62" t="s">
@@ -19736,21 +19780,21 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="111"/>
-      <c r="B125" s="105"/>
+      <c r="A125" s="113"/>
+      <c r="B125" s="107"/>
       <c r="C125" s="62" t="s">
         <v>1811</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="111"/>
-      <c r="B126" s="106"/>
+      <c r="A126" s="113"/>
+      <c r="B126" s="108"/>
       <c r="C126" s="62" t="s">
         <v>1812</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="112"/>
+      <c r="A127" s="114"/>
       <c r="B127" s="61" t="s">
         <v>160</v>
       </c>
@@ -19759,10 +19803,10 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="110" t="s">
+      <c r="A128" s="112" t="s">
         <v>1814</v>
       </c>
-      <c r="B128" s="104" t="s">
+      <c r="B128" s="106" t="s">
         <v>1815</v>
       </c>
       <c r="C128" s="62" t="s">
@@ -19770,36 +19814,36 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="111"/>
-      <c r="B129" s="105"/>
+      <c r="A129" s="113"/>
+      <c r="B129" s="107"/>
       <c r="C129" s="62" t="s">
         <v>1817</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="111"/>
-      <c r="B130" s="105"/>
+      <c r="A130" s="113"/>
+      <c r="B130" s="107"/>
       <c r="C130" s="62" t="s">
         <v>1818</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="111"/>
-      <c r="B131" s="105"/>
+      <c r="A131" s="113"/>
+      <c r="B131" s="107"/>
       <c r="C131" s="62" t="s">
         <v>1819</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="111"/>
-      <c r="B132" s="106"/>
+      <c r="A132" s="113"/>
+      <c r="B132" s="108"/>
       <c r="C132" s="62" t="s">
         <v>1820</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="111"/>
-      <c r="B133" s="104" t="s">
+      <c r="A133" s="113"/>
+      <c r="B133" s="106" t="s">
         <v>1821</v>
       </c>
       <c r="C133" s="62" t="s">
@@ -19807,29 +19851,29 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="111"/>
-      <c r="B134" s="105"/>
+      <c r="A134" s="113"/>
+      <c r="B134" s="107"/>
       <c r="C134" s="62" t="s">
         <v>1822</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="111"/>
-      <c r="B135" s="105"/>
+      <c r="A135" s="113"/>
+      <c r="B135" s="107"/>
       <c r="C135" s="62" t="s">
         <v>1823</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="111"/>
-      <c r="B136" s="106"/>
+      <c r="A136" s="113"/>
+      <c r="B136" s="108"/>
       <c r="C136" s="62" t="s">
         <v>1824</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="111"/>
-      <c r="B137" s="104" t="s">
+      <c r="A137" s="113"/>
+      <c r="B137" s="106" t="s">
         <v>1825</v>
       </c>
       <c r="C137" s="62" t="s">
@@ -19837,9 +19881,9 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="111"/>
-      <c r="B138" s="105"/>
-      <c r="C138" s="101" t="s">
+      <c r="A138" s="113"/>
+      <c r="B138" s="107"/>
+      <c r="C138" s="103" t="s">
         <v>1826</v>
       </c>
       <c r="D138" s="63" t="s">
@@ -19847,58 +19891,58 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="111"/>
-      <c r="B139" s="105"/>
-      <c r="C139" s="102"/>
+      <c r="A139" s="113"/>
+      <c r="B139" s="107"/>
+      <c r="C139" s="104"/>
       <c r="D139" s="63" t="s">
         <v>1827</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="111"/>
-      <c r="B140" s="105"/>
-      <c r="C140" s="102"/>
+      <c r="A140" s="113"/>
+      <c r="B140" s="107"/>
+      <c r="C140" s="104"/>
       <c r="D140" s="63" t="s">
         <v>1828</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="111"/>
-      <c r="B141" s="105"/>
-      <c r="C141" s="102"/>
+      <c r="A141" s="113"/>
+      <c r="B141" s="107"/>
+      <c r="C141" s="104"/>
       <c r="D141" s="63" t="s">
         <v>1829</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="111"/>
-      <c r="B142" s="105"/>
-      <c r="C142" s="102"/>
+      <c r="A142" s="113"/>
+      <c r="B142" s="107"/>
+      <c r="C142" s="104"/>
       <c r="D142" s="63" t="s">
         <v>1830</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="111"/>
-      <c r="B143" s="105"/>
-      <c r="C143" s="102"/>
+      <c r="A143" s="113"/>
+      <c r="B143" s="107"/>
+      <c r="C143" s="104"/>
       <c r="D143" s="63" t="s">
         <v>1831</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="111"/>
-      <c r="B144" s="105"/>
-      <c r="C144" s="102"/>
+      <c r="A144" s="113"/>
+      <c r="B144" s="107"/>
+      <c r="C144" s="104"/>
       <c r="D144" s="63" t="s">
         <v>1832</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="111"/>
-      <c r="B145" s="105"/>
-      <c r="C145" s="102"/>
-      <c r="D145" s="98" t="s">
+      <c r="A145" s="113"/>
+      <c r="B145" s="107"/>
+      <c r="C145" s="104"/>
+      <c r="D145" s="100" t="s">
         <v>1833</v>
       </c>
       <c r="E145" s="64" t="s">
@@ -19906,61 +19950,61 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="111"/>
-      <c r="B146" s="105"/>
-      <c r="C146" s="102"/>
-      <c r="D146" s="99"/>
+      <c r="A146" s="113"/>
+      <c r="B146" s="107"/>
+      <c r="C146" s="104"/>
+      <c r="D146" s="101"/>
       <c r="E146" s="64" t="s">
         <v>1834</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="111"/>
-      <c r="B147" s="105"/>
-      <c r="C147" s="102"/>
-      <c r="D147" s="99"/>
+      <c r="A147" s="113"/>
+      <c r="B147" s="107"/>
+      <c r="C147" s="104"/>
+      <c r="D147" s="101"/>
       <c r="E147" s="64" t="s">
         <v>1835</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="111"/>
-      <c r="B148" s="105"/>
-      <c r="C148" s="102"/>
-      <c r="D148" s="99"/>
+      <c r="A148" s="113"/>
+      <c r="B148" s="107"/>
+      <c r="C148" s="104"/>
+      <c r="D148" s="101"/>
       <c r="E148" s="64" t="s">
         <v>1836</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="111"/>
-      <c r="B149" s="105"/>
-      <c r="C149" s="102"/>
-      <c r="D149" s="100"/>
+      <c r="A149" s="113"/>
+      <c r="B149" s="107"/>
+      <c r="C149" s="104"/>
+      <c r="D149" s="102"/>
       <c r="E149" s="64" t="s">
         <v>1837</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="111"/>
-      <c r="B150" s="105"/>
-      <c r="C150" s="102"/>
+      <c r="A150" s="113"/>
+      <c r="B150" s="107"/>
+      <c r="C150" s="104"/>
       <c r="D150" s="63" t="s">
         <v>1838</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="111"/>
-      <c r="B151" s="105"/>
-      <c r="C151" s="103"/>
+      <c r="A151" s="113"/>
+      <c r="B151" s="107"/>
+      <c r="C151" s="105"/>
       <c r="D151" s="63" t="s">
         <v>1839</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="111"/>
-      <c r="B152" s="105"/>
-      <c r="C152" s="101" t="s">
+      <c r="A152" s="113"/>
+      <c r="B152" s="107"/>
+      <c r="C152" s="103" t="s">
         <v>1726</v>
       </c>
       <c r="D152" s="63" t="s">
@@ -19968,63 +20012,63 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="111"/>
-      <c r="B153" s="105"/>
-      <c r="C153" s="102"/>
+      <c r="A153" s="113"/>
+      <c r="B153" s="107"/>
+      <c r="C153" s="104"/>
       <c r="D153" s="63" t="s">
         <v>1840</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="111"/>
-      <c r="B154" s="105"/>
-      <c r="C154" s="102"/>
+      <c r="A154" s="113"/>
+      <c r="B154" s="107"/>
+      <c r="C154" s="104"/>
       <c r="D154" s="63" t="s">
         <v>1841</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="111"/>
-      <c r="B155" s="105"/>
-      <c r="C155" s="102"/>
+      <c r="A155" s="113"/>
+      <c r="B155" s="107"/>
+      <c r="C155" s="104"/>
       <c r="D155" s="63" t="s">
         <v>1842</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="111"/>
-      <c r="B156" s="105"/>
-      <c r="C156" s="102"/>
+      <c r="A156" s="113"/>
+      <c r="B156" s="107"/>
+      <c r="C156" s="104"/>
       <c r="D156" s="63" t="s">
         <v>1843</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="111"/>
-      <c r="B157" s="105"/>
-      <c r="C157" s="103"/>
+      <c r="A157" s="113"/>
+      <c r="B157" s="107"/>
+      <c r="C157" s="105"/>
       <c r="D157" s="63" t="s">
         <v>1844</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="111"/>
-      <c r="B158" s="105"/>
+      <c r="A158" s="113"/>
+      <c r="B158" s="107"/>
       <c r="C158" s="62" t="s">
         <v>1845</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="111"/>
-      <c r="B159" s="105"/>
+      <c r="A159" s="113"/>
+      <c r="B159" s="107"/>
       <c r="C159" s="62" t="s">
         <v>1846</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="111"/>
-      <c r="B160" s="105"/>
-      <c r="C160" s="101" t="s">
+      <c r="A160" s="113"/>
+      <c r="B160" s="107"/>
+      <c r="C160" s="103" t="s">
         <v>1861</v>
       </c>
       <c r="D160" s="63" t="s">
@@ -20032,10 +20076,10 @@
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="111"/>
-      <c r="B161" s="105"/>
-      <c r="C161" s="102"/>
-      <c r="D161" s="98" t="s">
+      <c r="A161" s="113"/>
+      <c r="B161" s="107"/>
+      <c r="C161" s="104"/>
+      <c r="D161" s="100" t="s">
         <v>1862</v>
       </c>
       <c r="E161" s="64" t="s">
@@ -20043,28 +20087,28 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="111"/>
-      <c r="B162" s="105"/>
-      <c r="C162" s="102"/>
-      <c r="D162" s="99"/>
+      <c r="A162" s="113"/>
+      <c r="B162" s="107"/>
+      <c r="C162" s="104"/>
+      <c r="D162" s="101"/>
       <c r="E162" s="64" t="s">
         <v>1864</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="111"/>
-      <c r="B163" s="105"/>
-      <c r="C163" s="102"/>
-      <c r="D163" s="100"/>
+      <c r="A163" s="113"/>
+      <c r="B163" s="107"/>
+      <c r="C163" s="104"/>
+      <c r="D163" s="102"/>
       <c r="E163" s="64" t="s">
         <v>1865</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="111"/>
-      <c r="B164" s="105"/>
-      <c r="C164" s="102"/>
-      <c r="D164" s="98" t="s">
+      <c r="A164" s="113"/>
+      <c r="B164" s="107"/>
+      <c r="C164" s="104"/>
+      <c r="D164" s="100" t="s">
         <v>1866</v>
       </c>
       <c r="E164" s="64" t="s">
@@ -20072,27 +20116,27 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="111"/>
-      <c r="B165" s="105"/>
-      <c r="C165" s="102"/>
-      <c r="D165" s="99"/>
+      <c r="A165" s="113"/>
+      <c r="B165" s="107"/>
+      <c r="C165" s="104"/>
+      <c r="D165" s="101"/>
       <c r="E165" s="64" t="s">
         <v>1867</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="111"/>
-      <c r="B166" s="105"/>
-      <c r="C166" s="103"/>
-      <c r="D166" s="100"/>
+      <c r="A166" s="113"/>
+      <c r="B166" s="107"/>
+      <c r="C166" s="105"/>
+      <c r="D166" s="102"/>
       <c r="E166" s="64" t="s">
         <v>1868</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="111"/>
-      <c r="B167" s="105"/>
-      <c r="C167" s="101" t="s">
+      <c r="A167" s="113"/>
+      <c r="B167" s="107"/>
+      <c r="C167" s="103" t="s">
         <v>1869</v>
       </c>
       <c r="D167" s="63" t="s">
@@ -20100,56 +20144,56 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="111"/>
-      <c r="B168" s="105"/>
-      <c r="C168" s="102"/>
+      <c r="A168" s="113"/>
+      <c r="B168" s="107"/>
+      <c r="C168" s="104"/>
       <c r="D168" s="63" t="s">
         <v>1870</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="111"/>
-      <c r="B169" s="105"/>
-      <c r="C169" s="102"/>
+      <c r="A169" s="113"/>
+      <c r="B169" s="107"/>
+      <c r="C169" s="104"/>
       <c r="D169" s="63" t="s">
         <v>1871</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="111"/>
-      <c r="B170" s="105"/>
-      <c r="C170" s="102"/>
+      <c r="A170" s="113"/>
+      <c r="B170" s="107"/>
+      <c r="C170" s="104"/>
       <c r="D170" s="63" t="s">
         <v>1872</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="111"/>
-      <c r="B171" s="105"/>
-      <c r="C171" s="102"/>
+      <c r="A171" s="113"/>
+      <c r="B171" s="107"/>
+      <c r="C171" s="104"/>
       <c r="D171" s="63" t="s">
         <v>1873</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="111"/>
-      <c r="B172" s="105"/>
-      <c r="C172" s="103"/>
+      <c r="A172" s="113"/>
+      <c r="B172" s="107"/>
+      <c r="C172" s="105"/>
       <c r="D172" s="63" t="s">
         <v>1874</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="111"/>
-      <c r="B173" s="105"/>
+      <c r="A173" s="113"/>
+      <c r="B173" s="107"/>
       <c r="C173" s="62" t="s">
         <v>1645</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="111"/>
-      <c r="B174" s="105"/>
-      <c r="C174" s="101" t="s">
+      <c r="A174" s="113"/>
+      <c r="B174" s="107"/>
+      <c r="C174" s="103" t="s">
         <v>1875</v>
       </c>
       <c r="D174" s="63" t="s">
@@ -20157,10 +20201,10 @@
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="111"/>
-      <c r="B175" s="105"/>
-      <c r="C175" s="102"/>
-      <c r="D175" s="98" t="s">
+      <c r="A175" s="113"/>
+      <c r="B175" s="107"/>
+      <c r="C175" s="104"/>
+      <c r="D175" s="100" t="s">
         <v>1876</v>
       </c>
       <c r="E175" s="64" t="s">
@@ -20168,73 +20212,73 @@
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="111"/>
-      <c r="B176" s="105"/>
-      <c r="C176" s="102"/>
-      <c r="D176" s="99"/>
+      <c r="A176" s="113"/>
+      <c r="B176" s="107"/>
+      <c r="C176" s="104"/>
+      <c r="D176" s="101"/>
       <c r="E176" s="64" t="s">
         <v>1878</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="111"/>
-      <c r="B177" s="105"/>
-      <c r="C177" s="102"/>
-      <c r="D177" s="99"/>
+      <c r="A177" s="113"/>
+      <c r="B177" s="107"/>
+      <c r="C177" s="104"/>
+      <c r="D177" s="101"/>
       <c r="E177" s="64" t="s">
         <v>1879</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="111"/>
-      <c r="B178" s="105"/>
-      <c r="C178" s="102"/>
-      <c r="D178" s="99"/>
+      <c r="A178" s="113"/>
+      <c r="B178" s="107"/>
+      <c r="C178" s="104"/>
+      <c r="D178" s="101"/>
       <c r="E178" s="64" t="s">
         <v>1880</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="111"/>
-      <c r="B179" s="105"/>
-      <c r="C179" s="102"/>
-      <c r="D179" s="99"/>
+      <c r="A179" s="113"/>
+      <c r="B179" s="107"/>
+      <c r="C179" s="104"/>
+      <c r="D179" s="101"/>
       <c r="E179" s="64" t="s">
         <v>1881</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="111"/>
-      <c r="B180" s="105"/>
-      <c r="C180" s="102"/>
-      <c r="D180" s="99"/>
+      <c r="A180" s="113"/>
+      <c r="B180" s="107"/>
+      <c r="C180" s="104"/>
+      <c r="D180" s="101"/>
       <c r="E180" s="64" t="s">
         <v>1882</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="111"/>
-      <c r="B181" s="105"/>
-      <c r="C181" s="102"/>
-      <c r="D181" s="99"/>
+      <c r="A181" s="113"/>
+      <c r="B181" s="107"/>
+      <c r="C181" s="104"/>
+      <c r="D181" s="101"/>
       <c r="E181" s="64" t="s">
         <v>1883</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="111"/>
-      <c r="B182" s="105"/>
-      <c r="C182" s="102"/>
-      <c r="D182" s="100"/>
+      <c r="A182" s="113"/>
+      <c r="B182" s="107"/>
+      <c r="C182" s="104"/>
+      <c r="D182" s="102"/>
       <c r="E182" s="64" t="s">
         <v>1884</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="111"/>
-      <c r="B183" s="105"/>
-      <c r="C183" s="102"/>
-      <c r="D183" s="98" t="s">
+      <c r="A183" s="113"/>
+      <c r="B183" s="107"/>
+      <c r="C183" s="104"/>
+      <c r="D183" s="100" t="s">
         <v>1885</v>
       </c>
       <c r="E183" s="64" t="s">
@@ -20242,154 +20286,154 @@
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="111"/>
-      <c r="B184" s="105"/>
-      <c r="C184" s="102"/>
-      <c r="D184" s="99"/>
+      <c r="A184" s="113"/>
+      <c r="B184" s="107"/>
+      <c r="C184" s="104"/>
+      <c r="D184" s="101"/>
       <c r="E184" s="64" t="s">
         <v>1886</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="111"/>
-      <c r="B185" s="105"/>
-      <c r="C185" s="102"/>
-      <c r="D185" s="99"/>
+      <c r="A185" s="113"/>
+      <c r="B185" s="107"/>
+      <c r="C185" s="104"/>
+      <c r="D185" s="101"/>
       <c r="E185" s="64" t="s">
         <v>1887</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="111"/>
-      <c r="B186" s="105"/>
-      <c r="C186" s="102"/>
-      <c r="D186" s="99"/>
+      <c r="A186" s="113"/>
+      <c r="B186" s="107"/>
+      <c r="C186" s="104"/>
+      <c r="D186" s="101"/>
       <c r="E186" s="64" t="s">
         <v>1888</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="111"/>
-      <c r="B187" s="105"/>
-      <c r="C187" s="102"/>
-      <c r="D187" s="99"/>
+      <c r="A187" s="113"/>
+      <c r="B187" s="107"/>
+      <c r="C187" s="104"/>
+      <c r="D187" s="101"/>
       <c r="E187" s="64" t="s">
         <v>1889</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="111"/>
-      <c r="B188" s="105"/>
-      <c r="C188" s="102"/>
-      <c r="D188" s="99"/>
+      <c r="A188" s="113"/>
+      <c r="B188" s="107"/>
+      <c r="C188" s="104"/>
+      <c r="D188" s="101"/>
       <c r="E188" s="64" t="s">
         <v>1890</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="111"/>
-      <c r="B189" s="105"/>
-      <c r="C189" s="102"/>
-      <c r="D189" s="99"/>
+      <c r="A189" s="113"/>
+      <c r="B189" s="107"/>
+      <c r="C189" s="104"/>
+      <c r="D189" s="101"/>
       <c r="E189" s="64" t="s">
         <v>1891</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="111"/>
-      <c r="B190" s="105"/>
-      <c r="C190" s="102"/>
-      <c r="D190" s="99"/>
+      <c r="A190" s="113"/>
+      <c r="B190" s="107"/>
+      <c r="C190" s="104"/>
+      <c r="D190" s="101"/>
       <c r="E190" s="64" t="s">
         <v>1892</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="111"/>
-      <c r="B191" s="105"/>
-      <c r="C191" s="102"/>
-      <c r="D191" s="99"/>
+      <c r="A191" s="113"/>
+      <c r="B191" s="107"/>
+      <c r="C191" s="104"/>
+      <c r="D191" s="101"/>
       <c r="E191" s="64" t="s">
         <v>1893</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="111"/>
-      <c r="B192" s="105"/>
-      <c r="C192" s="102"/>
-      <c r="D192" s="99"/>
+      <c r="A192" s="113"/>
+      <c r="B192" s="107"/>
+      <c r="C192" s="104"/>
+      <c r="D192" s="101"/>
       <c r="E192" s="64" t="s">
         <v>1894</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="111"/>
-      <c r="B193" s="105"/>
-      <c r="C193" s="102"/>
-      <c r="D193" s="99"/>
+      <c r="A193" s="113"/>
+      <c r="B193" s="107"/>
+      <c r="C193" s="104"/>
+      <c r="D193" s="101"/>
       <c r="E193" s="64" t="s">
         <v>1895</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="111"/>
-      <c r="B194" s="105"/>
-      <c r="C194" s="102"/>
-      <c r="D194" s="99"/>
+      <c r="A194" s="113"/>
+      <c r="B194" s="107"/>
+      <c r="C194" s="104"/>
+      <c r="D194" s="101"/>
       <c r="E194" s="64" t="s">
         <v>1896</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="111"/>
-      <c r="B195" s="105"/>
-      <c r="C195" s="102"/>
-      <c r="D195" s="99"/>
+      <c r="A195" s="113"/>
+      <c r="B195" s="107"/>
+      <c r="C195" s="104"/>
+      <c r="D195" s="101"/>
       <c r="E195" s="64" t="s">
         <v>1897</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="111"/>
-      <c r="B196" s="105"/>
-      <c r="C196" s="102"/>
-      <c r="D196" s="99"/>
+      <c r="A196" s="113"/>
+      <c r="B196" s="107"/>
+      <c r="C196" s="104"/>
+      <c r="D196" s="101"/>
       <c r="E196" s="64" t="s">
         <v>1898</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="111"/>
-      <c r="B197" s="105"/>
-      <c r="C197" s="102"/>
-      <c r="D197" s="99"/>
+      <c r="A197" s="113"/>
+      <c r="B197" s="107"/>
+      <c r="C197" s="104"/>
+      <c r="D197" s="101"/>
       <c r="E197" s="64" t="s">
         <v>1899</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="111"/>
-      <c r="B198" s="105"/>
-      <c r="C198" s="102"/>
-      <c r="D198" s="99"/>
+      <c r="A198" s="113"/>
+      <c r="B198" s="107"/>
+      <c r="C198" s="104"/>
+      <c r="D198" s="101"/>
       <c r="E198" s="64" t="s">
         <v>1900</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="111"/>
-      <c r="B199" s="105"/>
-      <c r="C199" s="102"/>
-      <c r="D199" s="100"/>
+      <c r="A199" s="113"/>
+      <c r="B199" s="107"/>
+      <c r="C199" s="104"/>
+      <c r="D199" s="102"/>
       <c r="E199" s="64" t="s">
         <v>1901</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="111"/>
-      <c r="B200" s="105"/>
-      <c r="C200" s="102"/>
-      <c r="D200" s="98" t="s">
+      <c r="A200" s="113"/>
+      <c r="B200" s="107"/>
+      <c r="C200" s="104"/>
+      <c r="D200" s="100" t="s">
         <v>1902</v>
       </c>
       <c r="E200" s="64" t="s">
@@ -20397,20 +20441,20 @@
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="111"/>
-      <c r="B201" s="105"/>
-      <c r="C201" s="102"/>
-      <c r="D201" s="99"/>
+      <c r="A201" s="113"/>
+      <c r="B201" s="107"/>
+      <c r="C201" s="104"/>
+      <c r="D201" s="101"/>
       <c r="E201" s="64" t="s">
         <v>1903</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="111"/>
-      <c r="B202" s="105"/>
-      <c r="C202" s="102"/>
-      <c r="D202" s="99"/>
-      <c r="E202" s="107" t="s">
+      <c r="A202" s="113"/>
+      <c r="B202" s="107"/>
+      <c r="C202" s="104"/>
+      <c r="D202" s="101"/>
+      <c r="E202" s="109" t="s">
         <v>1904</v>
       </c>
       <c r="F202" s="65" t="s">
@@ -20418,149 +20462,149 @@
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="111"/>
-      <c r="B203" s="105"/>
-      <c r="C203" s="102"/>
-      <c r="D203" s="99"/>
-      <c r="E203" s="108"/>
+      <c r="A203" s="113"/>
+      <c r="B203" s="107"/>
+      <c r="C203" s="104"/>
+      <c r="D203" s="101"/>
+      <c r="E203" s="110"/>
       <c r="F203" s="65" t="s">
         <v>1907</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="111"/>
-      <c r="B204" s="105"/>
-      <c r="C204" s="102"/>
-      <c r="D204" s="99"/>
-      <c r="E204" s="108"/>
+      <c r="A204" s="113"/>
+      <c r="B204" s="107"/>
+      <c r="C204" s="104"/>
+      <c r="D204" s="101"/>
+      <c r="E204" s="110"/>
       <c r="F204" s="65" t="s">
         <v>1906</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="111"/>
-      <c r="B205" s="105"/>
-      <c r="C205" s="102"/>
-      <c r="D205" s="99"/>
-      <c r="E205" s="108"/>
+      <c r="A205" s="113"/>
+      <c r="B205" s="107"/>
+      <c r="C205" s="104"/>
+      <c r="D205" s="101"/>
+      <c r="E205" s="110"/>
       <c r="F205" s="65" t="s">
         <v>1908</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="111"/>
-      <c r="B206" s="105"/>
-      <c r="C206" s="102"/>
-      <c r="D206" s="99"/>
-      <c r="E206" s="108"/>
+      <c r="A206" s="113"/>
+      <c r="B206" s="107"/>
+      <c r="C206" s="104"/>
+      <c r="D206" s="101"/>
+      <c r="E206" s="110"/>
       <c r="F206" s="65" t="s">
         <v>1909</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="111"/>
-      <c r="B207" s="105"/>
-      <c r="C207" s="102"/>
-      <c r="D207" s="99"/>
-      <c r="E207" s="108"/>
+      <c r="A207" s="113"/>
+      <c r="B207" s="107"/>
+      <c r="C207" s="104"/>
+      <c r="D207" s="101"/>
+      <c r="E207" s="110"/>
       <c r="F207" s="65" t="s">
         <v>1910</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="111"/>
-      <c r="B208" s="105"/>
-      <c r="C208" s="102"/>
-      <c r="D208" s="99"/>
-      <c r="E208" s="108"/>
+      <c r="A208" s="113"/>
+      <c r="B208" s="107"/>
+      <c r="C208" s="104"/>
+      <c r="D208" s="101"/>
+      <c r="E208" s="110"/>
       <c r="F208" s="65" t="s">
         <v>1911</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="111"/>
-      <c r="B209" s="105"/>
-      <c r="C209" s="102"/>
-      <c r="D209" s="99"/>
-      <c r="E209" s="108"/>
+      <c r="A209" s="113"/>
+      <c r="B209" s="107"/>
+      <c r="C209" s="104"/>
+      <c r="D209" s="101"/>
+      <c r="E209" s="110"/>
       <c r="F209" s="65" t="s">
         <v>1912</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="111"/>
-      <c r="B210" s="105"/>
-      <c r="C210" s="102"/>
-      <c r="D210" s="99"/>
-      <c r="E210" s="108"/>
+      <c r="A210" s="113"/>
+      <c r="B210" s="107"/>
+      <c r="C210" s="104"/>
+      <c r="D210" s="101"/>
+      <c r="E210" s="110"/>
       <c r="F210" s="65" t="s">
         <v>1913</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="111"/>
-      <c r="B211" s="105"/>
-      <c r="C211" s="102"/>
-      <c r="D211" s="99"/>
-      <c r="E211" s="108"/>
+      <c r="A211" s="113"/>
+      <c r="B211" s="107"/>
+      <c r="C211" s="104"/>
+      <c r="D211" s="101"/>
+      <c r="E211" s="110"/>
       <c r="F211" s="65" t="s">
         <v>1914</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="111"/>
-      <c r="B212" s="105"/>
-      <c r="C212" s="102"/>
-      <c r="D212" s="99"/>
-      <c r="E212" s="108"/>
+      <c r="A212" s="113"/>
+      <c r="B212" s="107"/>
+      <c r="C212" s="104"/>
+      <c r="D212" s="101"/>
+      <c r="E212" s="110"/>
       <c r="F212" s="65" t="s">
         <v>1915</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="111"/>
-      <c r="B213" s="105"/>
-      <c r="C213" s="102"/>
-      <c r="D213" s="99"/>
-      <c r="E213" s="108"/>
+      <c r="A213" s="113"/>
+      <c r="B213" s="107"/>
+      <c r="C213" s="104"/>
+      <c r="D213" s="101"/>
+      <c r="E213" s="110"/>
       <c r="F213" s="65" t="s">
         <v>1916</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="111"/>
-      <c r="B214" s="105"/>
-      <c r="C214" s="102"/>
-      <c r="D214" s="99"/>
-      <c r="E214" s="109"/>
+      <c r="A214" s="113"/>
+      <c r="B214" s="107"/>
+      <c r="C214" s="104"/>
+      <c r="D214" s="101"/>
+      <c r="E214" s="111"/>
       <c r="F214" s="65" t="s">
         <v>1917</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="111"/>
-      <c r="B215" s="105"/>
-      <c r="C215" s="102"/>
-      <c r="D215" s="99"/>
+      <c r="A215" s="113"/>
+      <c r="B215" s="107"/>
+      <c r="C215" s="104"/>
+      <c r="D215" s="101"/>
       <c r="E215" s="64" t="s">
         <v>1918</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="111"/>
-      <c r="B216" s="105"/>
-      <c r="C216" s="102"/>
-      <c r="D216" s="99"/>
+      <c r="A216" s="113"/>
+      <c r="B216" s="107"/>
+      <c r="C216" s="104"/>
+      <c r="D216" s="101"/>
       <c r="E216" s="64" t="s">
         <v>1919</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="111"/>
-      <c r="B217" s="105"/>
-      <c r="C217" s="102"/>
-      <c r="D217" s="99"/>
-      <c r="E217" s="107" t="s">
+      <c r="A217" s="113"/>
+      <c r="B217" s="107"/>
+      <c r="C217" s="104"/>
+      <c r="D217" s="101"/>
+      <c r="E217" s="109" t="s">
         <v>1920</v>
       </c>
       <c r="F217" s="65" t="s">
@@ -20568,97 +20612,97 @@
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="111"/>
-      <c r="B218" s="105"/>
-      <c r="C218" s="102"/>
-      <c r="D218" s="99"/>
-      <c r="E218" s="108"/>
+      <c r="A218" s="113"/>
+      <c r="B218" s="107"/>
+      <c r="C218" s="104"/>
+      <c r="D218" s="101"/>
+      <c r="E218" s="110"/>
       <c r="F218" s="65" t="s">
         <v>1921</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="111"/>
-      <c r="B219" s="105"/>
-      <c r="C219" s="102"/>
-      <c r="D219" s="99"/>
-      <c r="E219" s="108"/>
+      <c r="A219" s="113"/>
+      <c r="B219" s="107"/>
+      <c r="C219" s="104"/>
+      <c r="D219" s="101"/>
+      <c r="E219" s="110"/>
       <c r="F219" s="65" t="s">
         <v>1922</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="111"/>
-      <c r="B220" s="105"/>
-      <c r="C220" s="102"/>
-      <c r="D220" s="99"/>
-      <c r="E220" s="108"/>
+      <c r="A220" s="113"/>
+      <c r="B220" s="107"/>
+      <c r="C220" s="104"/>
+      <c r="D220" s="101"/>
+      <c r="E220" s="110"/>
       <c r="F220" s="65" t="s">
         <v>1923</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="111"/>
-      <c r="B221" s="105"/>
-      <c r="C221" s="102"/>
-      <c r="D221" s="99"/>
-      <c r="E221" s="108"/>
+      <c r="A221" s="113"/>
+      <c r="B221" s="107"/>
+      <c r="C221" s="104"/>
+      <c r="D221" s="101"/>
+      <c r="E221" s="110"/>
       <c r="F221" s="65" t="s">
         <v>1924</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="111"/>
-      <c r="B222" s="105"/>
-      <c r="C222" s="102"/>
-      <c r="D222" s="99"/>
-      <c r="E222" s="108"/>
+      <c r="A222" s="113"/>
+      <c r="B222" s="107"/>
+      <c r="C222" s="104"/>
+      <c r="D222" s="101"/>
+      <c r="E222" s="110"/>
       <c r="F222" s="65" t="s">
         <v>1925</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="111"/>
-      <c r="B223" s="105"/>
-      <c r="C223" s="102"/>
-      <c r="D223" s="99"/>
-      <c r="E223" s="108"/>
+      <c r="A223" s="113"/>
+      <c r="B223" s="107"/>
+      <c r="C223" s="104"/>
+      <c r="D223" s="101"/>
+      <c r="E223" s="110"/>
       <c r="F223" s="65" t="s">
         <v>1926</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="111"/>
-      <c r="B224" s="105"/>
-      <c r="C224" s="102"/>
-      <c r="D224" s="99"/>
-      <c r="E224" s="109"/>
+      <c r="A224" s="113"/>
+      <c r="B224" s="107"/>
+      <c r="C224" s="104"/>
+      <c r="D224" s="101"/>
+      <c r="E224" s="111"/>
       <c r="F224" s="65" t="s">
         <v>1927</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" s="111"/>
-      <c r="B225" s="105"/>
-      <c r="C225" s="102"/>
-      <c r="D225" s="99"/>
+      <c r="A225" s="113"/>
+      <c r="B225" s="107"/>
+      <c r="C225" s="104"/>
+      <c r="D225" s="101"/>
       <c r="E225" s="64" t="s">
         <v>1928</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" s="111"/>
-      <c r="B226" s="105"/>
-      <c r="C226" s="102"/>
-      <c r="D226" s="100"/>
+      <c r="A226" s="113"/>
+      <c r="B226" s="107"/>
+      <c r="C226" s="104"/>
+      <c r="D226" s="102"/>
       <c r="E226" s="64" t="s">
         <v>1929</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A227" s="112"/>
-      <c r="B227" s="106"/>
-      <c r="C227" s="103"/>
+      <c r="A227" s="114"/>
+      <c r="B227" s="108"/>
+      <c r="C227" s="105"/>
       <c r="D227" s="73" t="s">
         <v>1930</v>
       </c>
@@ -21782,13 +21826,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>2057</v>
       </c>
-      <c r="B1" s="116"/>
+      <c r="B1" s="118"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="117" t="s">
         <v>1853</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -21796,43 +21840,43 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="115"/>
+      <c r="A3" s="117"/>
       <c r="B3" s="2" t="s">
         <v>2059</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="115"/>
+      <c r="A4" s="117"/>
       <c r="B4" s="2" t="s">
         <v>2060</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="115"/>
+      <c r="A5" s="117"/>
       <c r="B5" s="2" t="s">
         <v>2061</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="115"/>
+      <c r="A6" s="117"/>
       <c r="B6" s="2" t="s">
         <v>2062</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="115"/>
+      <c r="A7" s="117"/>
       <c r="B7" s="2" t="s">
         <v>2063</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="115"/>
+      <c r="A8" s="117"/>
       <c r="B8" s="2" t="s">
         <v>2064</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="117" t="s">
         <v>1849</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -21840,43 +21884,43 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="115"/>
+      <c r="A10" s="117"/>
       <c r="B10" s="2" t="s">
         <v>2059</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="115"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="2" t="s">
         <v>2060</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="115"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="2" t="s">
         <v>2061</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="115"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="2" t="s">
         <v>2062</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="115"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="2" t="s">
         <v>2063</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="115"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="2" t="s">
         <v>2064</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="117" t="s">
         <v>2065</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -21884,43 +21928,43 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="115"/>
+      <c r="A17" s="117"/>
       <c r="B17" s="2" t="s">
         <v>2059</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="115"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="2" t="s">
         <v>2060</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="115"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="2" t="s">
         <v>2061</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="115"/>
+      <c r="A20" s="117"/>
       <c r="B20" s="2" t="s">
         <v>2062</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="115"/>
+      <c r="A21" s="117"/>
       <c r="B21" s="2" t="s">
         <v>2063</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="115"/>
+      <c r="A22" s="117"/>
       <c r="B22" s="2" t="s">
         <v>2064</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="115" t="s">
+      <c r="A23" s="117" t="s">
         <v>1485</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -21928,37 +21972,37 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="115"/>
+      <c r="A24" s="117"/>
       <c r="B24" s="2" t="s">
         <v>2059</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="115"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="2" t="s">
         <v>2060</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="115"/>
+      <c r="A26" s="117"/>
       <c r="B26" s="2" t="s">
         <v>2061</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="115"/>
+      <c r="A27" s="117"/>
       <c r="B27" s="2" t="s">
         <v>2062</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="115"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="2" t="s">
         <v>2063</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="115"/>
+      <c r="A29" s="117"/>
       <c r="B29" s="2" t="s">
         <v>2064</v>
       </c>

</xml_diff>